<commit_message>
tracking down mongodb error
</commit_message>
<xml_diff>
--- a/backend/receipts.xlsx
+++ b/backend/receipts.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -532,9 +532,35 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Matthew Wolz</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Greg s</v>
+      </c>
+      <c r="C6" t="str">
+        <v>3/24/2025</v>
+      </c>
+      <c r="D6" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Daily Guest Pass</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating the project. fixing a ton of functionality
</commit_message>
<xml_diff>
--- a/backend/receipts.xlsx
+++ b/backend/receipts.xlsx
@@ -397,46 +397,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Sponsor Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v xml:space="preserve"> Guest Name</v>
-      </c>
-      <c r="C1" t="str">
-        <v xml:space="preserve"> Date Sold</v>
-      </c>
-      <c r="D1" t="str">
-        <v xml:space="preserve"> SRC Staff Initials</v>
-      </c>
-      <c r="E1" t="str">
-        <v xml:space="preserve"> Guest Pass Number</v>
-      </c>
-      <c r="F1" t="str">
-        <v xml:space="preserve"> Email</v>
-      </c>
-      <c r="G1" t="str">
-        <v xml:space="preserve"> Product</v>
-      </c>
-      <c r="H1" t="str">
-        <v xml:space="preserve"> Amount</v>
-      </c>
-    </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Matthew Wolz</v>
       </c>
       <c r="B2" t="str">
-        <v>Greg S</v>
+        <v xml:space="preserve">JJ </v>
       </c>
       <c r="C2" t="str">
-        <v>3/24/2025</v>
+        <v>4/23/2025</v>
       </c>
       <c r="D2" t="str">
         <v>MW</v>
@@ -456,19 +430,19 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Matthew Wolz</v>
+        <v>Matthew wolz</v>
       </c>
       <c r="B3" t="str">
-        <v>Greg S</v>
+        <v>JJ</v>
       </c>
       <c r="C3" t="str">
-        <v>3/24/2025</v>
+        <v>4/23/2025</v>
       </c>
       <c r="D3" t="str">
         <v>MW</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F3" t="str">
         <v>N/A</v>
@@ -477,90 +451,12 @@
         <v>Daily Guest Pass</v>
       </c>
       <c r="H3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Matthew Wolz</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Greg S</v>
-      </c>
-      <c r="C4" t="str">
-        <v>3/24/2025</v>
-      </c>
-      <c r="D4" t="str">
-        <v>MW</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Daily Guest Pass</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Matthew Wolz</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Greg S</v>
-      </c>
-      <c r="C5" t="str">
-        <v>3/24/2025</v>
-      </c>
-      <c r="D5" t="str">
-        <v>MW</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Daily Guest Pass</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Matthew Wolz</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Greg s</v>
-      </c>
-      <c r="C6" t="str">
-        <v>3/24/2025</v>
-      </c>
-      <c r="D6" t="str">
-        <v>MW</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Daily Guest Pass</v>
-      </c>
-      <c r="H6">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding excel and receipt functionality
</commit_message>
<xml_diff>
--- a/backend/receipts.xlsx
+++ b/backend/receipts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-04-23" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -402,21 +402,47 @@
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Sponsor Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Guest Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Initials</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Receipt Number</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Item</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Price</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Matthew Wolz</v>
       </c>
       <c r="B2" t="str">
-        <v xml:space="preserve">JJ </v>
+        <v>Tiffany</v>
       </c>
       <c r="C2" t="str">
-        <v>4/23/2025</v>
+        <v>2025-04-23</v>
       </c>
       <c r="D2" t="str">
         <v>MW</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F2" t="str">
         <v>N/A</v>
@@ -430,19 +456,19 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Matthew wolz</v>
+        <v>Matthew Wolz</v>
       </c>
       <c r="B3" t="str">
-        <v>JJ</v>
+        <v>JJ James JJ</v>
       </c>
       <c r="C3" t="str">
-        <v>4/23/2025</v>
+        <v>2025-04-23</v>
       </c>
       <c r="D3" t="str">
         <v>MW</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F3" t="str">
         <v>N/A</v>

</xml_diff>

<commit_message>
updating a lot of components. main functionality is nearly complete
</commit_message>
<xml_diff>
--- a/backend/receipts.xlsx
+++ b/backend/receipts.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="2025-04-23" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-04-24" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-04-25" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -433,16 +434,16 @@
         <v>Matthew Wolz</v>
       </c>
       <c r="B2" t="str">
-        <v>Tiffany</v>
+        <v>Charles Darwin TESTING TWO</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-04-23</v>
+        <v>2025-04-24</v>
       </c>
       <c r="D2" t="str">
         <v>MW</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F2" t="str">
         <v>N/A</v>
@@ -459,16 +460,16 @@
         <v>Matthew Wolz</v>
       </c>
       <c r="B3" t="str">
-        <v>JJ James JJ</v>
+        <v>Justina Wimer</v>
       </c>
       <c r="C3" t="str">
-        <v>2025-04-23</v>
+        <v>2025-04-24</v>
       </c>
       <c r="D3" t="str">
         <v>MW</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F3" t="str">
         <v>N/A</v>
@@ -480,9 +481,309 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Matthew Wolz</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Justina Wimer</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2025-04-24</v>
+      </c>
+      <c r="D4" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Daily Guest Pass</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>James W</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Greg S</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-04-24</v>
+      </c>
+      <c r="D5" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G5" t="str">
+        <v>10 Visit Guest Pass</v>
+      </c>
+      <c r="H5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Tiffany Neff</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2025-04-24</v>
+      </c>
+      <c r="D6" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G6" t="str">
+        <v>10 Visit Children Guest Pass</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Kafi Rahman</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Little Kafi Rahman</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2025-04-24</v>
+      </c>
+      <c r="D7" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Youth Guest Pass</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Charles Darwin</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Isaac Newton</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2025-04-24</v>
+      </c>
+      <c r="D8" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Youth Guest Pass</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Matthew Wolz</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Aiden W</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-04-24</v>
+      </c>
+      <c r="D9" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Daily Guest Pass</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Matthew Wolz</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Mason Berliner</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2025-04-24</v>
+      </c>
+      <c r="D10" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Daily Guest Pass</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Sponsor Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Guest Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Initials</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Receipt Number</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Item</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Price</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>matthew wolz</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Adli Jacobs</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2025-04-25</v>
+      </c>
+      <c r="D2" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Daily Guest Pass</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Matthew Wolz</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Aiden Wolz</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2025-04-25</v>
+      </c>
+      <c r="D3" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Youth Guest Pass</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>matthew wolz</v>
+      </c>
+      <c r="B4" t="str">
+        <v>jj something</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2025-04-25</v>
+      </c>
+      <c r="D4" t="str">
+        <v>MW</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Youth Guest Pass</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>